<commit_message>
thanhvv: commit code base & docs
</commit_message>
<xml_diff>
--- a/Du an Tieng anh giao tiep mien phi.xlsx
+++ b/Du an Tieng anh giao tiep mien phi.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanhvv/Documents/ThanhVV11/03. Công việc/01. Dự án cá nhân/02.TiengAnhGiaoTiepMienPhi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B27BA0-D11B-2241-B448-48F9C9B9115D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F632A8B-98DB-6840-A270-BDD9D269184B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="27360" windowHeight="17740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12940" yWindow="1500" windowWidth="19600" windowHeight="17740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chức năng chính" sheetId="57" r:id="rId1"/>
     <sheet name="TECH STACK" sheetId="60" r:id="rId2"/>
+    <sheet name="Database" sheetId="61" r:id="rId3"/>
+    <sheet name="Kiến trúc login" sheetId="62" r:id="rId4"/>
+    <sheet name="Cơ chế" sheetId="63" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="387">
   <si>
     <t>Auth Service</t>
   </si>
@@ -709,6 +712,829 @@
   </si>
   <si>
     <t>Load Balancer → Gateway → Services</t>
+  </si>
+  <si>
+    <t>CREATE TABLE users (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  id BIGSERIAL PRIMARY KEY,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  email VARCHAR(150) UNIQUE NOT NULL,</t>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t>CREATE TABLE lessons (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  order_index INT,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  is_active BOOLEAN DEFAULT true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  sub_title VARCHAR(150),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  image VARCHAR(150),</t>
+  </si>
+  <si>
+    <t>CREATE TABLE lesson_contents (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  code VARCHAR(50) UNIQUE NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  title VARCHAR(150) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  level VARCHAR(50),</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  lesson_id BIGINT UNIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    REFERENCES lessons(id) ON DELETE CASCADE,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  content JSONB NOT NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  password VARCHAR(255) NOT NULL,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  full_name VARCHAR(150),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  avatar VARCHAR(255),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  role VARCHAR(50) NOT NULL, -- USER / ADMIN / CONTENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  is_active BOOLEAN DEFAULT true,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  created_at TIMESTAMP DEFAULT now(),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  updated_at TIMESTAMP DEFAULT now()</t>
+  </si>
+  <si>
+    <t>🔐 OVERVIEW — MÔ HÌNH AUTH TRONG HỆ THỐNG</t>
+  </si>
+  <si>
+    <t>1️⃣ Mục tiêu của mô hình auth</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>đăng nhập 1 lần</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dùng token để gọi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>toàn bộ hệ thống</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Các service </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KHÔNG tự xử lý login</t>
+    </r>
+  </si>
+  <si>
+    <t>Dễ mở rộng (JWT, OAuth2 sau này)</t>
+  </si>
+  <si>
+    <t>2️⃣ Các thành phần tham gia</t>
+  </si>
+  <si>
+    <t>[ Client / UI ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        v</t>
+  </si>
+  <si>
+    <t>[ API-GATEWAY ]</t>
+  </si>
+  <si>
+    <t>[ AUTH-SERVICE ]</t>
+  </si>
+  <si>
+    <t>Và khi đã login xong:</t>
+  </si>
+  <si>
+    <t>[ Client ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   |  JWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   v</t>
+  </si>
+  <si>
+    <t>[ API-GATEWAY ] ---&gt; [ LESSON / SPEAKING / OTHER SERVICE ]</t>
+  </si>
+  <si>
+    <t>3️⃣ Vai trò từng thành phần (rất quan trọng)</t>
+  </si>
+  <si>
+    <t>🔹 Auth Service</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">👉 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Trung tâm xác thực</t>
+    </r>
+  </si>
+  <si>
+    <t>Đăng ký (register)</t>
+  </si>
+  <si>
+    <t>Đăng nhập (login)</t>
+  </si>
+  <si>
+    <t>Validate username/password</t>
+  </si>
+  <si>
+    <t>Generate JWT</t>
+  </si>
+  <si>
+    <t>❌ Không xử lý business</t>
+  </si>
+  <si>
+    <t>❌ Không check JWT cho request khác</t>
+  </si>
+  <si>
+    <t>🔹 API Gateway</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">👉 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cổng bảo vệ hệ thống</t>
+    </r>
+  </si>
+  <si>
+    <t>Nhận request từ client</t>
+  </si>
+  <si>
+    <t>Check JWT (sau login)</t>
+  </si>
+  <si>
+    <t>Chặn request không hợp lệ</t>
+  </si>
+  <si>
+    <t>Forward request sang service</t>
+  </si>
+  <si>
+    <t>❌ Không login</t>
+  </si>
+  <si>
+    <t>❌ Không lưu user</t>
+  </si>
+  <si>
+    <t>🔹 Business Services (lesson, speaking,…)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">👉 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chỉ xử lý nghiệp vụ</t>
+    </r>
+  </si>
+  <si>
+    <t>Tin rằng request đã được gateway xác thực</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nhận </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>userId</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> từ header</t>
+    </r>
+  </si>
+  <si>
+    <t>Không biết gì về password / JWT</t>
+  </si>
+  <si>
+    <t>4️⃣ Auth Flow (luồng đăng nhập)</t>
+  </si>
+  <si>
+    <t>🔑 Login</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | POST /auth/login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  v</t>
+  </si>
+  <si>
+    <t>API-GATEWAY</t>
+  </si>
+  <si>
+    <t>AUTH-SERVICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | verify email + password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | generate JWT</t>
+  </si>
+  <si>
+    <t>Client (nhận JWT)</t>
+  </si>
+  <si>
+    <t>🔐 Gọi API sau khi login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | Authorization: Bearer &lt;JWT&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | verify JWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | extract userId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  | add header X-User-Id</t>
+  </si>
+  <si>
+    <t>LESSON / SPEAKING SERVICE</t>
+  </si>
+  <si>
+    <t>5️⃣ JWT dùng để làm gì?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">JWT chứa </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>thông tin tối thiểu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:</t>
+    </r>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "userId": 12,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "email": "boss@gmail.com",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "role": "USER"</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>👉 JWT dùng để:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Xác định </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ai đang gọi API</t>
+    </r>
+  </si>
+  <si>
+    <t>Phân quyền (USER / ADMIN)</t>
+  </si>
+  <si>
+    <t>Không cần query DB mỗi request</t>
+  </si>
+  <si>
+    <t>6️⃣ Vì sao Gateway check JWT, không phải Auth Service?</t>
+  </si>
+  <si>
+    <t>👉 Vì:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Auth Service chỉ nên làm </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>login</t>
+    </r>
+  </si>
+  <si>
+    <t>Nếu mọi request đều gọi Auth Service → bottleneck</t>
+  </si>
+  <si>
+    <t>Gateway là điểm vào → check 1 lần là đủ</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">📌 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Best practice microservice</t>
+    </r>
+  </si>
+  <si>
+    <t>7️⃣ Tại sao business service KHÔNG check JWT?</t>
+  </si>
+  <si>
+    <t>Tránh duplicate logic</t>
+  </si>
+  <si>
+    <t>Tránh share secret JWT</t>
+  </si>
+  <si>
+    <t>Service nhẹ, tập trung nghiệp vụ</t>
+  </si>
+  <si>
+    <t>👉 Gateway chịu trách nhiệm bảo vệ hệ thống</t>
+  </si>
+  <si>
+    <t>8️⃣ Path chuẩn trong mô hình auth</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Nơi xử lý</t>
+  </si>
+  <si>
+    <t>/auth/login</t>
+  </si>
+  <si>
+    <t>/auth/register</t>
+  </si>
+  <si>
+    <t>/lessons/**</t>
+  </si>
+  <si>
+    <t>/speaking/**</t>
+  </si>
+  <si>
+    <t>9️⃣ Những nguyên tắc “khắc cốt ghi tâm”</t>
+  </si>
+  <si>
+    <t>- Login chỉ có ở Auth Service</t>
+  </si>
+  <si>
+    <t>- JWT được verify ở API Gateway</t>
+  </si>
+  <si>
+    <t>- Business service tin Gateway</t>
+  </si>
+  <si>
+    <t>- Không gọi service trực tiếp</t>
+  </si>
+  <si>
+    <t>- Mọi request đi qua Gateway</t>
+  </si>
+  <si>
+    <t>🔥 TÓM TẮT CỰC NGẮN (COPY NOTE)</t>
+  </si>
+  <si>
+    <t>Auth Service: login + register + issue JWT</t>
+  </si>
+  <si>
+    <t>API Gateway: verify JWT + protect API</t>
+  </si>
+  <si>
+    <t>Business Service: xử lý nghiệp vụ, không auth</t>
+  </si>
+  <si>
+    <t>User login 1 lần, dùng JWT cho toàn hệ thống</t>
+  </si>
+  <si>
+    <t>Gateway là cổng bảo vệ duy nhất</t>
+  </si>
+  <si>
+    <t>🔐 OVERVIEW — SECURITY MODEL (MICROSERVICE)</t>
+  </si>
+  <si>
+    <t>1️⃣ Mục tiêu security</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Đăng nhập </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1 lần</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bảo vệ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>toàn bộ API</t>
+    </r>
+  </si>
+  <si>
+    <t>Không check security trùng lặp</t>
+  </si>
+  <si>
+    <t>Dễ mở rộng (role, OAuth2, refresh token)</t>
+  </si>
+  <si>
+    <t>2️⃣ Nguyên tắc cốt lõi (RẤT QUAN TRỌNG)</t>
+  </si>
+  <si>
+    <t>- Security tập trung tại API Gateway</t>
+  </si>
+  <si>
+    <t>- Auth Service chỉ dùng để login/register</t>
+  </si>
+  <si>
+    <t>- Business Service không xử lý security</t>
+  </si>
+  <si>
+    <t>- Mọi request bắt buộc đi qua Gateway</t>
+  </si>
+  <si>
+    <t>3️⃣ Các thành phần trong security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    v</t>
+  </si>
+  <si>
+    <t>[ API-GATEWAY ]  ← kiểm tra JWT, phân quyền</t>
+  </si>
+  <si>
+    <t>[ AUTH-SERVICE ] ← login, register, cấp JWT</t>
+  </si>
+  <si>
+    <t>[ BUSINESS SERVICE ] ← chỉ xử lý nghiệp vụ</t>
+  </si>
+  <si>
+    <t>4️⃣ Auth Service (Authentication)</t>
+  </si>
+  <si>
+    <t>Nhiệm vụ</t>
+  </si>
+  <si>
+    <t>Xác thực user bằng email/password</t>
+  </si>
+  <si>
+    <t>Hash password (BCrypt)</t>
+  </si>
+  <si>
+    <t>Không làm</t>
+  </si>
+  <si>
+    <t>Không verify JWT cho request khác</t>
+  </si>
+  <si>
+    <t>Không bảo vệ API business</t>
+  </si>
+  <si>
+    <t>API chính</t>
+  </si>
+  <si>
+    <t>POST /auth/login</t>
+  </si>
+  <si>
+    <t>POST /auth/register</t>
+  </si>
+  <si>
+    <t>5️⃣ JWT (Token dùng cho toàn hệ thống)</t>
+  </si>
+  <si>
+    <t>Nội dung JWT (payload tối thiểu)</t>
+  </si>
+  <si>
+    <t>Mục đích</t>
+  </si>
+  <si>
+    <t>Xác định người dùng</t>
+  </si>
+  <si>
+    <t>Phân quyền</t>
+  </si>
+  <si>
+    <t>6️⃣ API Gateway (Authorization)</t>
+  </si>
+  <si>
+    <t>Chặn request chưa login</t>
+  </si>
+  <si>
+    <t>Verify JWT (signature + expiration)</t>
+  </si>
+  <si>
+    <t>Extract thông tin user</t>
+  </si>
+  <si>
+    <t>Forward request hợp lệ</t>
+  </si>
+  <si>
+    <t>Cách hoạt động</t>
+  </si>
+  <si>
+    <t>Request</t>
+  </si>
+  <si>
+    <t>→ Check Authorization header</t>
+  </si>
+  <si>
+    <t>→ Verify JWT</t>
+  </si>
+  <si>
+    <t>→ Extract userId, role</t>
+  </si>
+  <si>
+    <t>→ Add header X-User-Id</t>
+  </si>
+  <si>
+    <t>→ Forward sang service</t>
+  </si>
+  <si>
+    <t>7️⃣ Business Service (Lesson, Speaking…)</t>
+  </si>
+  <si>
+    <t>Nhận request đã được xác thực</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dùng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>X-User-Id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> để xử lý logic</t>
+    </r>
+  </si>
+  <si>
+    <t>Không decode JWT</t>
+  </si>
+  <si>
+    <t>Không biết secret JWT</t>
+  </si>
+  <si>
+    <t>Không xử lý login</t>
+  </si>
+  <si>
+    <t>8️⃣ Phân quyền (Authorization)</t>
+  </si>
+  <si>
+    <t>Ví dụ rule</t>
+  </si>
+  <si>
+    <t>/auth/**        → public</t>
+  </si>
+  <si>
+    <t>/lessons/**     → USER</t>
+  </si>
+  <si>
+    <t>/admin/**       → ADMIN</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">👉 Rule này </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>đặt tại Gateway</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, không đặt trong service.</t>
+    </r>
+  </si>
+  <si>
+    <t>9️⃣ Vì sao không check JWT ở từng service?</t>
+  </si>
+  <si>
+    <t>Tránh share secret</t>
+  </si>
+  <si>
+    <t>Giảm coupling</t>
+  </si>
+  <si>
+    <t>Dễ maintain &amp; scale</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">👉 Gateway là </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>single security entry point</t>
+    </r>
+  </si>
+  <si>
+    <t>🔥 CHECKLIST SECURITY CHUẨN</t>
+  </si>
+  <si>
+    <t>- JWT chỉ được tạo ở Auth Service</t>
+  </si>
+  <si>
+    <t>- JWT chỉ được verify ở API Gateway</t>
+  </si>
+  <si>
+    <t>- Không dùng session</t>
+  </si>
+  <si>
+    <t>🧠 TÓM TẮT NGẮN GỌN (COPY NOTE)</t>
+  </si>
+  <si>
+    <t>Auth Service: login, register, issue JWT</t>
+  </si>
+  <si>
+    <t>API Gateway: verify JWT, authorize request</t>
+  </si>
+  <si>
+    <t>Business Service: xử lý nghiệp vụ</t>
+  </si>
+  <si>
+    <t>JWT dùng cho toàn hệ thống</t>
+  </si>
+  <si>
+    <t>Gateway là cổng bảo mật duy nhất</t>
   </si>
 </sst>
 </file>
@@ -1195,9 +2021,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
+    <sheetView topLeftCell="A12" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1705,8 +2529,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A122"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B128" sqref="A95:B128"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2021,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" ht="11" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>97</v>
       </c>
@@ -2325,4 +3149,1204 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CEC8C5-F449-D14E-9896-56E01C87042D}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C222361E-2EAA-6244-82C0-180D35ED1026}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:B109"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B94" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B95" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="B96" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B97" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2331897A-2FAF-D245-AFFC-CA56510F0B60}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:B88"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B51" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B52" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B54" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="24" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="16" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>